<commit_message>
Fix can not take cell when empty column exist #11
</commit_message>
<xml_diff>
--- a/tests/fixtures/test1.xlsx
+++ b/tests/fixtures/test1.xlsx
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -368,11 +368,11 @@
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1">
         <v>10</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix get shared strings with multi-formatted
</commit_message>
<xml_diff>
--- a/tests/fixtures/test1.xlsx
+++ b/tests/fixtures/test1.xlsx
@@ -1,19 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hashimoto/works/yama96/vendor/hhashimoto/excel-reader/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27400" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>sheetName</t>
     <phoneticPr fontId="1"/>
@@ -34,12 +45,35 @@
     <t>Sheet2</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>あいうえお</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +87,13 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic (本文)"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -357,23 +398,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
       <c r="C1">
         <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -390,12 +434,12 @@
       <selection activeCell="C3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -417,12 +461,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>

</xml_diff>